<commit_message>
Implemented feature no.7 - user permission management.
</commit_message>
<xml_diff>
--- a/Documentation/Product Management/Product features.xlsx
+++ b/Documentation/Product Management/Product features.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -118,9 +118,6 @@
     <t>log attempts in database and send via email when an error (or above) happens</t>
   </si>
   <si>
-    <t>be able to create, delete and edit other users. The simple users will only be able to edit their data (except from their category)</t>
-  </si>
-  <si>
     <t>to properly insert the organizational chart in the database</t>
   </si>
   <si>
@@ -134,9 +131,6 @@
   </si>
   <si>
     <t>login and use the application only if I am activated</t>
-  </si>
-  <si>
-    <t>be able to manage users (check product doc)</t>
   </si>
 </sst>
 </file>
@@ -556,7 +550,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>19</v>
@@ -644,7 +638,7 @@
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4" t="s">
@@ -682,21 +676,25 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+    <row r="7" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>7</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="C7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>32</v>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -704,18 +702,26 @@
         <v>8</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
         <v>9</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>37</v>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -809,10 +815,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,7 +843,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>19</v>
@@ -861,45 +867,17 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Started working on resource strings of templates
</commit_message>
<xml_diff>
--- a/Documentation/Product Management/Product features.xlsx
+++ b/Documentation/Product Management/Product features.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="product backlog" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
   <si>
     <t>ID</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>login and use the application only if I am activated</t>
+  </si>
+  <si>
+    <t>Fix form fields in user edit form. They show None</t>
   </si>
 </sst>
 </file>
@@ -525,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,9 +727,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>10</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -817,7 +823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Made some changes to the product documents and to the deleteuser.html template
</commit_message>
<xml_diff>
--- a/Documentation/Product Management/Product features.xlsx
+++ b/Documentation/Product Management/Product features.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="product backlog" sheetId="1" r:id="rId1"/>
@@ -528,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,18 +665,25 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+    <row r="6" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
         <v>6</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="F6" s="4"/>
+      <c r="G6" s="4" t="s">
         <v>30</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -727,12 +734,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+    <row r="10" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
         <v>10</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4" t="s">
         <v>37</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -823,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,18 +889,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created the organization sqlalchemy models. Created an initial organization blueprint (org) Restructured the code that puts initial data in the database
</commit_message>
<xml_diff>
--- a/Documentation/Product Management/Product features.xlsx
+++ b/Documentation/Product Management/Product features.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="product backlog" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
   <si>
     <t>ID</t>
   </si>
@@ -134,6 +134,24 @@
   </si>
   <si>
     <t>Fix form fields in user edit form. They show None</t>
+  </si>
+  <si>
+    <t>to see pdf reports for employees per department etc.</t>
+  </si>
+  <si>
+    <t>setup virtual environment for the app</t>
+  </si>
+  <si>
+    <t>it can be uploaded and run from servers</t>
+  </si>
+  <si>
+    <t>do some performance profiling for the application</t>
+  </si>
+  <si>
+    <t>it can be optimized</t>
+  </si>
+  <si>
+    <t>http://docs.sqlalchemy.org/en/rel_1_0/faq/performance.html#faq-how-to-profile</t>
   </si>
 </sst>
 </file>
@@ -528,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,19 +769,37 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E11" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>13</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -839,7 +875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changes to product features document
</commit_message>
<xml_diff>
--- a/Documentation/Product Management/Product features.xlsx
+++ b/Documentation/Product Management/Product features.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
   <si>
     <t>ID</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>http://docs.sqlalchemy.org/en/rel_1_0/faq/performance.html#faq-how-to-profile</t>
+  </si>
+  <si>
+    <t>improve code design usign design patterns</t>
   </si>
 </sst>
 </file>
@@ -547,7 +550,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -802,9 +805,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>14</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- Added functionality for editing organizations - Added functionality for deleting organizations
</commit_message>
<xml_diff>
--- a/Documentation/Product Management/Product features.xlsx
+++ b/Documentation/Product Management/Product features.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="47">
   <si>
     <t>ID</t>
   </si>
@@ -155,6 +155,12 @@
   </si>
   <si>
     <t>improve code design usign design patterns</t>
+  </si>
+  <si>
+    <t>Add irs number field to organization</t>
+  </si>
+  <si>
+    <t>Add constraints and messages to deletions (eg in organizations that have parent organizations)</t>
   </si>
 </sst>
 </file>
@@ -550,7 +556,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,10 +823,16 @@
       <c r="A15" s="3">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E15" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>16</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- Finished with the edit Service page - Restructured code. -- Add and edit service pages now use common code and html -- Add and edit organization pages now use common code and html
+ Finish code restructuring for employees
+ Solve problem when editing and saving an organization or service with empty name. Then, in the list empty names show up, but in the database everything is OK. Must be something related to db sessions.
</commit_message>
<xml_diff>
--- a/Documentation/Product Management/Product features.xlsx
+++ b/Documentation/Product Management/Product features.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="50">
   <si>
     <t>ID</t>
   </si>
@@ -161,6 +161,15 @@
   </si>
   <si>
     <t>Add constraints and messages to deletions (eg in organizations that have parent organizations)</t>
+  </si>
+  <si>
+    <t>add photo for users</t>
+  </si>
+  <si>
+    <t>add logo for organizations</t>
+  </si>
+  <si>
+    <t>delete View button on user form. Rename Επεξεργασία to Προβολή/Επεξεργασία</t>
   </si>
 </sst>
 </file>
@@ -556,7 +565,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,15 +795,23 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+    <row r="12" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
         <v>12</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="4" t="s">
         <v>40</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -811,12 +828,21 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+    <row r="14" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
         <v>14</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4" t="s">
         <v>44</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -835,42 +861,51 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E17" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E18" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E19" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>24</v>
       </c>
@@ -894,7 +929,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
- Installed various things on venv - Started working on image uploading. -- created new blueprint for uploads -- wrote code for uploading organization logos
+ add some bootstrap code to properly show images
+ continue with user photos
</commit_message>
<xml_diff>
--- a/Documentation/Product Management/Product features.xlsx
+++ b/Documentation/Product Management/Product features.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="product backlog" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="50">
   <si>
     <t>ID</t>
   </si>
@@ -564,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,12 +743,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+    <row r="8" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>8</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
         <v>32</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -926,10 +935,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,12 +987,28 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>32</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>18</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- started changing the html code (login and edit user form) related to the forms, according to the bootstrap website instructions.
</commit_message>
<xml_diff>
--- a/Documentation/Product Management/Product features.xlsx
+++ b/Documentation/Product Management/Product features.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="51">
   <si>
     <t>ID</t>
   </si>
@@ -169,7 +169,10 @@
     <t>add logo for organizations</t>
   </si>
   <si>
-    <t>delete View button on user form. Rename Επεξεργασία to Προβολή/Επεξεργασία</t>
+    <t>delete View button on user form. Rename Επεξεργασία to Προβολή/Επεξεργασία. Use readonly property</t>
+  </si>
+  <si>
+    <t>improve forms code according to bootstrap instructions</t>
   </si>
 </sst>
 </file>
@@ -564,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,18 +826,25 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+    <row r="13" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
         <v>13</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="4" t="s">
         <v>43</v>
+      </c>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -854,39 +864,75 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+    <row r="15" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
         <v>15</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
         <v>16</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>17</v>
-      </c>
-      <c r="E17" s="3" t="s">
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>17</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
         <v>18</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>19</v>
       </c>
@@ -894,27 +940,30 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>24</v>
       </c>
@@ -935,10 +984,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,36 +1036,28 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>18</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I3 I4:I1048576">
       <formula1>userstorystatus</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H3 H4:H1048576">
       <formula1>priority</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
- Started working on pdf reports creation.
</commit_message>
<xml_diff>
--- a/Documentation/Product Management/Product features.xlsx
+++ b/Documentation/Product Management/Product features.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="52">
   <si>
     <t>ID</t>
   </si>
@@ -173,6 +173,9 @@
   </si>
   <si>
     <t>improve forms code according to bootstrap instructions</t>
+  </si>
+  <si>
+    <t>enable oath 2 for authorization</t>
   </si>
 </sst>
 </file>
@@ -567,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD20"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,17 +943,29 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+    <row r="20" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
         <v>20</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4" t="s">
         <v>50</v>
+      </c>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>21</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -987,7 +1002,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,26 +1053,26 @@
     </row>
     <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I3 I4:I1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I1048576">
       <formula1>userstorystatus</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H3 H4:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576">
       <formula1>priority</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
- Started working on actions component
</commit_message>
<xml_diff>
--- a/Documentation/Product Management/Product features.xlsx
+++ b/Documentation/Product Management/Product features.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -176,6 +176,12 @@
   </si>
   <si>
     <t>enable oath 2 for authorization</t>
+  </si>
+  <si>
+    <t>create the projects list page and related functionality</t>
+  </si>
+  <si>
+    <t>create the project details form and related functionality</t>
   </si>
 </sst>
 </file>
@@ -571,7 +577,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+      <selection activeCell="A22" sqref="A22:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -802,12 +808,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+    <row r="11" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
         <v>11</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4" t="s">
         <v>38</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -968,14 +983,20 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E22" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>23</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1053,18 +1074,18 @@
     </row>
     <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>